<commit_message>
make minor fixes with extent report .info & addeddescription to testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="AddMultipleCustomer" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -153,7 +153,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
added excel utility with dataprovide
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="AddMultipleCustomer" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="addMultipleCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="openAccountTest" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,15 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">Fname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PinCode</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post Code</t>
   </si>
   <si>
     <t xml:space="preserve">Shiv</t>
@@ -47,6 +48,21 @@
   </si>
   <si>
     <t xml:space="preserve">176033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xyz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currency</t>
   </si>
 </sst>
 </file>
@@ -147,13 +163,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -186,6 +202,17 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -197,4 +224,36 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished writting framework, will make changes after some advice
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="addMultipleCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -47,10 +47,10 @@
     <t xml:space="preserve">3967</t>
   </si>
   <si>
-    <t xml:space="preserve">Keyword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Driven</t>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cust</t>
   </si>
   <si>
     <t xml:space="preserve">1332</t>
@@ -174,11 +174,11 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -242,11 +242,11 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.11"/>
   </cols>

</xml_diff>